<commit_message>
Updated text and catalogue files
</commit_message>
<xml_diff>
--- a/static/links-to-solo-for-the-art-kleiner-archive.xlsx
+++ b/static/links-to-solo-for-the-art-kleiner-archive.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Futures Library\Guidance for Researchers\Complete\Art Kleiner Archive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Futures Library\Workon\linked\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEAD111-A36C-4824-AF6D-B22EE1479B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{007E5D63-4C8A-4EC2-85F9-ECC3A11C20E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Art Kleiner Archive" sheetId="1" r:id="rId1"/>
+    <sheet name="SOLO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,182 +32,95 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>Item Numbers</t>
   </si>
   <si>
-    <t>Box 1.1</t>
-  </si>
-  <si>
     <t>1-37</t>
   </si>
   <si>
-    <t>Box 1.2</t>
-  </si>
-  <si>
     <t>38-99</t>
   </si>
   <si>
-    <t>Box 1.3</t>
-  </si>
-  <si>
     <t>100-125</t>
   </si>
   <si>
-    <t>Box 1.4</t>
-  </si>
-  <si>
     <t>126-151</t>
   </si>
   <si>
-    <t>Box 1.5</t>
-  </si>
-  <si>
     <t>152-202</t>
   </si>
   <si>
-    <t>Box 2.1</t>
-  </si>
-  <si>
     <t>203-258</t>
   </si>
   <si>
-    <t>Box 2.2</t>
-  </si>
-  <si>
     <t>259-321</t>
   </si>
   <si>
-    <t>Box 2.3</t>
-  </si>
-  <si>
     <t>322-347</t>
   </si>
   <si>
-    <t>Box 2.4</t>
-  </si>
-  <si>
     <t>348-389</t>
   </si>
   <si>
-    <t>Box 2.5</t>
-  </si>
-  <si>
     <t>390-443</t>
   </si>
   <si>
-    <t>Box 3.1</t>
-  </si>
-  <si>
     <t>444-478</t>
   </si>
   <si>
-    <t>Box 3.2</t>
-  </si>
-  <si>
     <t>479-520</t>
   </si>
   <si>
-    <t>Box 3.3</t>
-  </si>
-  <si>
     <t>521-588</t>
   </si>
   <si>
-    <t>Box 3.4</t>
-  </si>
-  <si>
     <t>589-652</t>
   </si>
   <si>
-    <t>Box 3.5</t>
-  </si>
-  <si>
     <t>653-688</t>
   </si>
   <si>
-    <t>Box 4.1</t>
-  </si>
-  <si>
     <t>689-723</t>
   </si>
   <si>
-    <t>Box 4.2</t>
-  </si>
-  <si>
     <t>724-769</t>
   </si>
   <si>
-    <t>Box 4.3</t>
-  </si>
-  <si>
     <t>770-829</t>
   </si>
   <si>
-    <t>Box 4.4</t>
-  </si>
-  <si>
     <t>830-886</t>
   </si>
   <si>
-    <t>Box 4.5</t>
-  </si>
-  <si>
     <t>887-959</t>
   </si>
   <si>
-    <t>Box 5.1</t>
-  </si>
-  <si>
     <t>960-1033</t>
   </si>
   <si>
-    <t>Box 5.2</t>
-  </si>
-  <si>
     <t>1034-1114</t>
   </si>
   <si>
-    <t>Box 5.3</t>
-  </si>
-  <si>
     <t>1115-1156</t>
   </si>
   <si>
-    <t>Box 5.4</t>
-  </si>
-  <si>
     <t>1157-1211</t>
   </si>
   <si>
-    <t>Box 5.5</t>
-  </si>
-  <si>
     <t>1212-1249</t>
   </si>
   <si>
-    <t>Box 6.1</t>
-  </si>
-  <si>
     <t>1250-1308</t>
   </si>
   <si>
-    <t>Box 6.2</t>
-  </si>
-  <si>
     <t>1309-1365</t>
   </si>
   <si>
-    <t>Box 6.3</t>
-  </si>
-  <si>
     <t>1366-1441</t>
   </si>
   <si>
-    <t>Box 6.4</t>
-  </si>
-  <si>
     <t>1442-1507</t>
   </si>
   <si>
@@ -214,13 +128,286 @@
   </si>
   <si>
     <t>Please refer to 'The Art Kleiner Archive: A Descriptive Catalogue' (2016), for item descriptions.</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>SOLO</t>
+  </si>
+  <si>
+    <t>Box number</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 1.1</t>
+  </si>
+  <si>
+    <t>308643785</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676450107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 1.2</t>
+  </si>
+  <si>
+    <t>308643786</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676460107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 1.3</t>
+  </si>
+  <si>
+    <t>308643782</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676420107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 1.4</t>
+  </si>
+  <si>
+    <t>308643783</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676430107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 1.5</t>
+  </si>
+  <si>
+    <t>308643784</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676440107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 2.1</t>
+  </si>
+  <si>
+    <t>308643788</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676480107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 2.2</t>
+  </si>
+  <si>
+    <t>308643530</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226643690107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 2.3</t>
+  </si>
+  <si>
+    <t>308643779</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226643870107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 2.4</t>
+  </si>
+  <si>
+    <t>308643780</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226643900107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 2.5</t>
+  </si>
+  <si>
+    <t>308643787</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676490107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 3.1</t>
+  </si>
+  <si>
+    <t>308643789</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676500107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 3.2</t>
+  </si>
+  <si>
+    <t>308643790</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676520107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 3.3</t>
+  </si>
+  <si>
+    <t>308643791</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676530107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 3.4</t>
+  </si>
+  <si>
+    <t>308643792</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676540107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 3.5</t>
+  </si>
+  <si>
+    <t>308643793</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676560107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 4.1</t>
+  </si>
+  <si>
+    <t>308643794</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676580107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 4.2</t>
+  </si>
+  <si>
+    <t>308643795</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676590107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 4.3</t>
+  </si>
+  <si>
+    <t>308643796</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676600107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 4.4</t>
+  </si>
+  <si>
+    <t>308643797</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676620107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 4.5</t>
+  </si>
+  <si>
+    <t>308643798</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676630107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 5.1</t>
+  </si>
+  <si>
+    <t>308643799</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676640107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 5.2</t>
+  </si>
+  <si>
+    <t>308643800</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676660107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 5.3</t>
+  </si>
+  <si>
+    <t>308643801</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676670107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 5.4</t>
+  </si>
+  <si>
+    <t>308643802</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226676680107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 5.5</t>
+  </si>
+  <si>
+    <t>308643803</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226686090107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 6.1</t>
+  </si>
+  <si>
+    <t>308643804</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226686100107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 6.2</t>
+  </si>
+  <si>
+    <t>308643805</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226686120107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 6.3</t>
+  </si>
+  <si>
+    <t>308643806</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226686140107026</t>
+  </si>
+  <si>
+    <t>Oxford Futures Library. Art Kleiner Archive. Box 6.4</t>
+  </si>
+  <si>
+    <t>308643807</t>
+  </si>
+  <si>
+    <t>https://solo.bodleian.ox.ac.uk/permalink/44OXF_INST/35n82s/alma990226686160107026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,8 +439,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +464,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,11 +488,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
@@ -296,21 +508,6 @@
       </left>
       <right style="medium">
         <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -324,19 +521,6 @@
       </left>
       <right style="medium">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -356,8 +540,8 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -366,25 +550,53 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -396,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -404,31 +616,40 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -739,311 +960,795 @@
   <dimension ref="B2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="2:6" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="2" spans="2:6" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="13">
+        <f>HYPERLINK(SOLO!C2,SOLO!D2)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <f>HYPERLINK(SOLO!C3,SOLO!D3)</f>
+        <v>1.2</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="8" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <f>HYPERLINK(SOLO!C4,SOLO!D4)</f>
+        <v>1.3</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <f>HYPERLINK(SOLO!C5,SOLO!D5)</f>
+        <v>1.4</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="8" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <f>HYPERLINK(SOLO!C6,SOLO!D6)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="9" t="s">
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
+        <f>HYPERLINK(SOLO!C7,SOLO!D7)</f>
+        <v>2.1</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="8" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <f>HYPERLINK(SOLO!C8,SOLO!D8)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9" t="s">
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
+        <f>HYPERLINK(SOLO!C9,SOLO!D9)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="8" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
+        <f>HYPERLINK(SOLO!C10,SOLO!D10)</f>
+        <v>2.4</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9" t="s">
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="11">
+        <f>HYPERLINK(SOLO!C11,SOLO!D11)</f>
+        <v>2.5</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="8" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
+        <f>HYPERLINK(SOLO!C12,SOLO!D12)</f>
+        <v>3.1</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="9" t="s">
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
+        <f>HYPERLINK(SOLO!C13,SOLO!D13)</f>
+        <v>3.2</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="8" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="11">
+        <f>HYPERLINK(SOLO!C14,SOLO!D14)</f>
+        <v>3.3</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="9" t="s">
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <f>HYPERLINK(SOLO!C15,SOLO!D15)</f>
+        <v>3.4</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="8" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="11">
+        <f>HYPERLINK(SOLO!C16,SOLO!D16)</f>
+        <v>3.5</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="9" t="s">
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="11">
+        <f>HYPERLINK(SOLO!C17,SOLO!D17)</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="8" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
+        <f>HYPERLINK(SOLO!C18,SOLO!D18)</f>
+        <v>4.2</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="9" t="s">
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="11">
+        <f>HYPERLINK(SOLO!C19,SOLO!D19)</f>
+        <v>4.3</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="8" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
+        <f>HYPERLINK(SOLO!C20,SOLO!D20)</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="9" t="s">
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
+        <f>HYPERLINK(SOLO!C21,SOLO!D21)</f>
+        <v>4.5</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="8" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <f>HYPERLINK(SOLO!C22,SOLO!D22)</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="9" t="s">
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <f>HYPERLINK(SOLO!C23,SOLO!D23)</f>
+        <v>5.2</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="8" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <f>HYPERLINK(SOLO!C24,SOLO!D24)</f>
+        <v>5.3</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="9" t="s">
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
+        <f>HYPERLINK(SOLO!C25,SOLO!D25)</f>
+        <v>5.4</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="8" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
+        <f>HYPERLINK(SOLO!C26,SOLO!D26)</f>
+        <v>5.5</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="9" t="s">
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="11">
+        <f>HYPERLINK(SOLO!C27,SOLO!D27)</f>
+        <v>6.1</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="8" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="11">
+        <f>HYPERLINK(SOLO!C28,SOLO!D28)</f>
+        <v>6.2</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="9" t="s">
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="11">
+        <f>HYPERLINK(SOLO!C29,SOLO!D29)</f>
+        <v>6.3</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="8" t="s">
+    <row r="33" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="12">
+        <f>HYPERLINK(SOLO!C30,SOLO!D30)</f>
+        <v>6.4</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{6247139D-1D47-4911-B4A8-1CEE32BF7FD2}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{3433194B-CAE1-4208-A69D-F8E815C1F81B}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{FC77A592-30DE-43FB-BCFE-76D074BF4B45}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{3C4567DE-26A1-4DA8-8B5E-DD2DA5F88807}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{0211C896-DFAC-4BBD-A52C-EC4B5DEC67F1}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{472DF09B-E5BB-48C8-8FEA-CF5C24FB531E}"/>
-    <hyperlink ref="B11" r:id="rId7" xr:uid="{94F94DBD-8958-4F43-AE9F-BAE76DA66E98}"/>
-    <hyperlink ref="B12" r:id="rId8" xr:uid="{F60F6848-6F1C-4DB7-90F1-3D3B573B0E8D}"/>
-    <hyperlink ref="B13" r:id="rId9" xr:uid="{9594DD54-88AA-416F-BA7C-B520BB5DE5F0}"/>
-    <hyperlink ref="B14" r:id="rId10" xr:uid="{8FB8AC8F-53EE-45E7-870D-8F53C5106B04}"/>
-    <hyperlink ref="B15" r:id="rId11" xr:uid="{850C0EBC-1EFF-4B65-AEBF-33755FF4F74D}"/>
-    <hyperlink ref="B16" r:id="rId12" xr:uid="{E2623009-6E1C-4BFB-A883-ED7A0D192745}"/>
-    <hyperlink ref="B17" r:id="rId13" xr:uid="{0304A40C-ABE4-4E7F-9BF9-C339B5158149}"/>
-    <hyperlink ref="B18" r:id="rId14" xr:uid="{FF556A87-DB34-49A2-887B-B6F89BC47711}"/>
-    <hyperlink ref="B19" r:id="rId15" xr:uid="{83FC6914-C911-4839-AD9A-1CAB67C94019}"/>
-    <hyperlink ref="B20" r:id="rId16" xr:uid="{0DD36EF6-642F-44E2-AA2E-815FB261B48E}"/>
-    <hyperlink ref="B21" r:id="rId17" xr:uid="{0E16BD26-696A-474D-A4C0-D5E4224F73FE}"/>
-    <hyperlink ref="B22" r:id="rId18" xr:uid="{21AB055B-9039-42DA-9136-6F7529D29536}"/>
-    <hyperlink ref="B23" r:id="rId19" xr:uid="{F9920D95-93B3-4C59-A9B1-C38962117401}"/>
-    <hyperlink ref="B24" r:id="rId20" xr:uid="{BD911424-40CB-413D-8214-D70596F0EBB7}"/>
-    <hyperlink ref="B25" r:id="rId21" xr:uid="{3EA22078-004B-4D89-ACBC-6C24BD05BA6F}"/>
-    <hyperlink ref="B26" r:id="rId22" xr:uid="{81350F3B-FAB7-40B8-895D-495406655FEF}"/>
-    <hyperlink ref="B27" r:id="rId23" xr:uid="{6E8FD711-4679-404E-BA67-8888F1EA1AFB}"/>
-    <hyperlink ref="B28" r:id="rId24" xr:uid="{A502226B-AA62-4015-8D3B-858C81675FDF}"/>
-    <hyperlink ref="B29" r:id="rId25" xr:uid="{56317DA2-AAEA-4D42-83C6-5F4F7CFD5E70}"/>
-    <hyperlink ref="B30" r:id="rId26" xr:uid="{570A69A6-48AF-44F1-9426-BAB92C83721B}"/>
-    <hyperlink ref="B31" r:id="rId27" xr:uid="{0FD09CF0-DC0C-450D-BD30-9E8E8BC39F5E}"/>
-    <hyperlink ref="B32" r:id="rId28" xr:uid="{FDC84C3B-F4E3-4812-B846-6A05A177ED8D}"/>
-    <hyperlink ref="B33" r:id="rId29" xr:uid="{F78FF7D9-8FA0-45F6-829C-92C467E822C5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="C5" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C78F65-B80A-4111-A08F-7F91CBD14A95}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30">
+        <v>6.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{61D4B6DC-AAF4-4076-ABAD-559663FCECE1}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{57F48872-0F90-42FC-8A31-0C7B5B264C57}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{75BD8AE0-D5D6-4535-842D-B8005F4AB5CD}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{977F4514-CB77-48CF-B044-0FAF1E77E9CA}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{1FE69B29-3C2F-429E-A78F-2EE37B0F8A2A}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{D2F9CF99-02AE-4412-944B-4878A8A33606}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{25DC1E12-ABB4-4EC6-A2E1-C03A29EC0528}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{59CD3FEA-5464-453A-A868-0BAAC1D779AF}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{C3F2C490-6014-49A6-BE0B-50CDF19B2F5C}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{EC94F06F-6EB0-4484-ABCC-FD748E7B3972}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{C277801A-F67F-4978-8608-F47FA9295EE3}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{415610CF-83D5-409C-B3DD-568A08623136}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{514D92AE-02FE-4411-94BD-E58591B282FE}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{8B29D0EA-CBB0-4454-828C-4A2D43E1877C}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{630DD1A5-B2B3-4A53-9FEE-63AFE1134B38}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{0F792D80-BC32-4A97-BF8F-5D07613939FD}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{0723D29C-073E-46B4-98A3-5C942D4FA339}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{3D748C38-FDD2-4AB8-ABEA-7D06AB999056}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{23B78A11-61A0-42AC-9494-D4C057E63612}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{444CA308-ED2B-4CE4-96A7-73A322933805}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{3A7DEE90-B6B0-40A0-880D-C03BEBED6AE9}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{642A4B9A-26C2-4F32-B2E5-FB9FBF96CD3A}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{118DB778-44A5-4458-8CE0-DF434FA513AA}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{59A5FCA8-427F-4DAF-AA83-D3A578430782}"/>
+    <hyperlink ref="C26" r:id="rId25" xr:uid="{6DF742C3-DE0B-4364-87FC-F7C9FC774A8E}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{860BA9DD-F920-4D6D-A254-570AA27E0AAA}"/>
+    <hyperlink ref="C28" r:id="rId27" xr:uid="{A01DD35F-182B-4778-ADF6-377E4545E7AB}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{F6341077-B498-48F4-B0B4-ED876D7866A4}"/>
+    <hyperlink ref="C30" r:id="rId29" xr:uid="{8B50C8CB-407D-4687-AA96-54CF0D5CAA72}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088A0D7DC92D19A4FB78A3764798821D1" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5b5bbd72790895a483193971c6b0572">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6f1281f-7111-4d7e-97ca-f7eabed4923f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="97f527103aeb5feae6d5fdcd5b1609c9" ns2:_="">
     <xsd:import namespace="f6f1281f-7111-4d7e-97ca-f7eabed4923f"/>
@@ -1215,22 +1920,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C3A09E3-2DCB-4F3A-840C-A9F6350B33F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3642EBF-6EDB-471B-9203-6F3F33DE94D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5D9AE12-5A49-4832-A11F-7AAB8ECB4A10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1246,21 +1953,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3642EBF-6EDB-471B-9203-6F3F33DE94D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C3A09E3-2DCB-4F3A-840C-A9F6350B33F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>